<commit_message>
include series 100 to 999
</commit_message>
<xml_diff>
--- a/Cash Voucher/bin/Debug/res/Cash Voucher.xlsx
+++ b/Cash Voucher/bin/Debug/res/Cash Voucher.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmmc\Documents\Visual Studio 2008\Projects\Cash Voucher\Cash Voucher\bin\Debug\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cash Voucher\Cash Voucher\bin\Debug\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Voucher" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +592,14 @@
       <b/>
       <sz val="28"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -751,12 +759,63 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -770,60 +829,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,7 +1136,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E5"/>
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,102 +1151,102 @@
   <sheetData>
     <row r="1" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
       <c r="G4" t="s">
         <v>2</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="24"/>
+      <c r="I4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
       <c r="G5" t="s">
         <v>3</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="23"/>
+      <c r="I5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="B6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="18"/>
+      <c r="A9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1434,22 +1447,22 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="13"/>
+      <c r="A21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1461,136 +1474,139 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="G24" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
+      <c r="A24" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="22">
+      <c r="B28" s="19">
         <f>B4</f>
         <v>0</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
       <c r="G28" t="s">
         <v>2</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
       </c>
-      <c r="I28" s="20" t="str">
+      <c r="I28" s="26" t="str">
         <f>I4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J28" s="20"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
       <c r="G29" t="s">
         <v>3</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
       </c>
-      <c r="I29" s="23" t="str">
+      <c r="I29" s="5" t="str">
         <f>I5</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J29" s="23"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>174</v>
       </c>
-      <c r="B30" s="7" t="str">
+      <c r="B30" s="24" t="str">
         <f>B6</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="str">
+      <c r="A33" s="11" t="str">
         <f>A9</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="16" t="str">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="11" t="str">
         <f>F9</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="16" t="str">
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="11" t="str">
         <f>I9</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J33" s="18"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="str">
@@ -1824,59 +1840,133 @@
       <c r="J44" s="10"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="str">
+      <c r="A45" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="11" t="str">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="11" t="str">
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="14" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J45" s="13"/>
+      <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>7</v>
       </c>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
       <c r="G47" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="str">
+      <c r="A48" s="21" t="str">
         <f>A24</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="G48" s="5" t="str">
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="22" t="str">
         <f>G24</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="B4:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="B28:E29"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:E21"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A10:E10"/>
@@ -1893,81 +1983,13 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="B28:E29"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:E5"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>